<commit_message>
New complement assay plot, new combined (DLS-Zeta-Pico) plot
</commit_message>
<xml_diff>
--- a/CellUptake_Plots/Cell Uptake_Aryelle Experiment_02.09.2024/20240209_CellUptake_DIPLibrary.xlsx
+++ b/CellUptake_Plots/Cell Uptake_Aryelle Experiment_02.09.2024/20240209_CellUptake_DIPLibrary.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryellewright/Documents/Documents - Aryelle’s MacBook Air/Kumar-Biomaterials-Lab/CellUptake_Plots/Cell Uptake_Aryelle Experiment_02.09.2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBF29DA-239C-2246-BEB6-3C2EC98972CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC72CB2-3919-D245-B374-9E0129F859F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27900" yWindow="1460" windowWidth="25040" windowHeight="14820" activeTab="1" xr2:uid="{6A097125-46FF-5B48-8771-77A19FC4ECD4}"/>
+    <workbookView xWindow="6860" yWindow="1840" windowWidth="25040" windowHeight="14820" activeTab="2" xr2:uid="{6A097125-46FF-5B48-8771-77A19FC4ECD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="14">
   <si>
     <t>Sample</t>
   </si>
@@ -73,19 +74,37 @@
   </si>
   <si>
     <t>G3</t>
+  </si>
+  <si>
+    <t>N/P ratio</t>
+  </si>
+  <si>
+    <t>pDNA+
+H₂O</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -96,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -104,12 +123,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,7 +471,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B6" sqref="B6:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -551,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98151F63-8C73-C64D-B551-1C8B9D66DF10}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -670,4 +714,312 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1866DCDB-AFD5-C44B-93BE-4B1B31F70E9E}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>137.14523333333332</v>
+      </c>
+      <c r="D2">
+        <v>3.0774642960290151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>5355.0865999999996</v>
+      </c>
+      <c r="D3">
+        <v>65.317215750290345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>144757.95853333335</v>
+      </c>
+      <c r="D4">
+        <v>7849.7811571914235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>75569.738200000007</v>
+      </c>
+      <c r="D5">
+        <v>3851.2502215658369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>58099.1708</v>
+      </c>
+      <c r="D7">
+        <v>7819.285162300409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="C8">
+        <v>59722.09426666666</v>
+      </c>
+      <c r="D8">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>8881.6723666666658</v>
+      </c>
+      <c r="D11">
+        <v>210.77546624890473</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="C12">
+        <v>11842.476433333331</v>
+      </c>
+      <c r="D12">
+        <v>898.8833893182383</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>38433.3079</v>
+      </c>
+      <c r="D15">
+        <v>5514.9746228541198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="C16">
+        <v>38763.979266666669</v>
+      </c>
+      <c r="D16">
+        <v>6310.2056450739401</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="3">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>41633.498299999999</v>
+      </c>
+      <c r="D19">
+        <v>7051.7939644152484</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="C20">
+        <v>30772.651633333327</v>
+      </c>
+      <c r="D20">
+        <v>4367.1110222270918</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="3">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>26767.266033333333</v>
+      </c>
+      <c r="D23">
+        <v>4520.1206988648892</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="C24">
+        <v>21410.490333333331</v>
+      </c>
+      <c r="D24">
+        <v>1685.4500277749723</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="3">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Editing the shapes in my scatter plot to distinguish polymer type
</commit_message>
<xml_diff>
--- a/CellUptake_Plots/Cell Uptake_Aryelle Experiment_02.09.2024/20240209_CellUptake_DIPLibrary.xlsx
+++ b/CellUptake_Plots/Cell Uptake_Aryelle Experiment_02.09.2024/20240209_CellUptake_DIPLibrary.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryellewright/Documents/Documents - Aryelle’s MacBook Air/Kumar-Biomaterials-Lab/CellUptake_Plots/Cell Uptake_Aryelle Experiment_02.09.2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC72CB2-3919-D245-B374-9E0129F859F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289279BD-C847-2F41-96E0-49EB171F6B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6860" yWindow="1840" windowWidth="25040" windowHeight="14820" activeTab="2" xr2:uid="{6A097125-46FF-5B48-8771-77A19FC4ECD4}"/>
+    <workbookView xWindow="15860" yWindow="4460" windowWidth="19620" windowHeight="15000" activeTab="2" xr2:uid="{6A097125-46FF-5B48-8771-77A19FC4ECD4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="NP-1" sheetId="1" r:id="rId1"/>
+    <sheet name="NP-10" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="59">
   <si>
     <t>Sample</t>
   </si>
@@ -76,11 +76,145 @@
     <t>G3</t>
   </si>
   <si>
-    <t>N/P ratio</t>
-  </si>
-  <si>
-    <t>pDNA+
-H₂O</t>
+    <t>Polymer</t>
+  </si>
+  <si>
+    <t>N/P Ratio</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>Sample Name</t>
+  </si>
+  <si>
+    <t>Geometric Mean</t>
+  </si>
+  <si>
+    <t>A1 G3-10-1</t>
+  </si>
+  <si>
+    <t>A1 UT-1</t>
+  </si>
+  <si>
+    <t>A2 G3-10-2</t>
+  </si>
+  <si>
+    <t>A2 UT-2</t>
+  </si>
+  <si>
+    <t>A3 G3-10-3</t>
+  </si>
+  <si>
+    <t>A3 UT-3</t>
+  </si>
+  <si>
+    <t>A4 pDNA-CELLSCRUB-1</t>
+  </si>
+  <si>
+    <t>A5 pDNA-CELLSCRUB-2</t>
+  </si>
+  <si>
+    <t>A6 pDNA-LOTION-3</t>
+  </si>
+  <si>
+    <t>A7 LPF-1</t>
+  </si>
+  <si>
+    <t>A8 LPF-2</t>
+  </si>
+  <si>
+    <t>B1 LPF-3</t>
+  </si>
+  <si>
+    <t>B2 J-1</t>
+  </si>
+  <si>
+    <t>B3 J-2</t>
+  </si>
+  <si>
+    <t>B4 J-3</t>
+  </si>
+  <si>
+    <t>B5 S1-1</t>
+  </si>
+  <si>
+    <t>B6 S1-2</t>
+  </si>
+  <si>
+    <t>B7 S1-3</t>
+  </si>
+  <si>
+    <t>B8 B1-1</t>
+  </si>
+  <si>
+    <t>C1 B1-2</t>
+  </si>
+  <si>
+    <t>C2 B1-3</t>
+  </si>
+  <si>
+    <t>C3 G1-1-1</t>
+  </si>
+  <si>
+    <t>C4 G1-1-2</t>
+  </si>
+  <si>
+    <t>C5 G1-1-3</t>
+  </si>
+  <si>
+    <t>C6 G2-1-1</t>
+  </si>
+  <si>
+    <t>C7 G2-1-2</t>
+  </si>
+  <si>
+    <t>C8 G2-1-3</t>
+  </si>
+  <si>
+    <t>D1 G3-1-1</t>
+  </si>
+  <si>
+    <t>D2 G3-1-2</t>
+  </si>
+  <si>
+    <t>D3 G3-1-3</t>
+  </si>
+  <si>
+    <t>D4 S10-1</t>
+  </si>
+  <si>
+    <t>D5 S10-2</t>
+  </si>
+  <si>
+    <t>D6 S10-3</t>
+  </si>
+  <si>
+    <t>D7 B10-1</t>
+  </si>
+  <si>
+    <t>D8 B10-2</t>
+  </si>
+  <si>
+    <t>E1 B10-3</t>
+  </si>
+  <si>
+    <t>E2 G1-10-1</t>
+  </si>
+  <si>
+    <t>E3 G1-10-2</t>
+  </si>
+  <si>
+    <t>E4 G1-10-3</t>
+  </si>
+  <si>
+    <t>E5 G2-10-1</t>
+  </si>
+  <si>
+    <t>E6 G2-10-2</t>
+  </si>
+  <si>
+    <t>E7 G2-10-3</t>
   </si>
 </sst>
 </file>
@@ -101,10 +235,11 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,7 +250,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -123,37 +258,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,15 +580,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B717E6A3-332C-6948-9E8D-96CAFABA57DB}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C10"/>
+      <selection activeCell="A6" sqref="A6:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="18.83203125" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,104 +602,446 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>137.14523333333332</v>
+        <f>AVERAGE(H3+H5+H7)</f>
+        <v>534.08280000000002</v>
       </c>
       <c r="C2">
-        <v>3.0774642960290151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <f>STDEV(H3,H5,H7)</f>
+        <v>3.8624421199546837</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2">
+        <v>55899.412199999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>5355.0865999999996</v>
+        <f>AVERAGE(H8+H9+H10)</f>
+        <v>15596.172400000001</v>
       </c>
       <c r="C3">
-        <v>65.317215750290345</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <f>STDEV(H8:H10)</f>
+        <v>788.03543538336555</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>180.4204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>144757.95853333335</v>
+        <f>AVERAGE(H14:H16)</f>
+        <v>382599.03173333331</v>
       </c>
       <c r="C4">
-        <v>7849.7811571914235</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <f>STDEV(H14:H16)</f>
+        <v>30668.289784134882</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4">
+        <v>71341.169699999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>75569.738200000007</v>
+        <f>AVERAGE(H11:H13)</f>
+        <v>78788.300500000012</v>
       </c>
       <c r="C5">
-        <v>3851.2502215658369</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <f>STDEV(H11:H13)</f>
+        <v>11900.014254468426</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>173.57169999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>58099.1708</v>
+        <f>AVERAGE(H17:H19)</f>
+        <v>21758.752600000003</v>
       </c>
       <c r="C6">
-        <v>7819.285162300409</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <f>STDEV(H17:H19)</f>
+        <v>768.24076767646204</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6">
+        <v>77272.876000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>8881.6723666666658</v>
+        <f>AVERAGE(H20:H22)</f>
+        <v>8222.9890000000014</v>
       </c>
       <c r="C7">
-        <v>210.77546624890473</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <f>STDEV(H20:H22)</f>
+        <v>53.309537557645477</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7">
+        <v>180.0907</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>38433.3079</v>
+        <f>AVERAGE(H23:H25)</f>
+        <v>10353.305133333333</v>
       </c>
       <c r="C8">
-        <v>5514.9746228541198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <f>STDEV(H23:H25)</f>
+        <v>964.45757572783066</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8">
+        <v>5386.1584999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
-        <v>41633.498299999999</v>
+        <f>AVERAGE(H26:H28)</f>
+        <v>12865.843566666668</v>
       </c>
       <c r="C9">
-        <v>7051.7939644152484</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <f>STDEV(H26:H28)</f>
+        <v>1360.9383822682871</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9">
+        <v>4333.8707000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>26767.266033333333</v>
+        <f>AVERAGE(H29:H31)</f>
+        <v>11194.053699999999</v>
       </c>
       <c r="C10">
-        <v>4520.1206988648892</v>
+        <f>STDEV(H29:H31)</f>
+        <v>331.24462803304402</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10">
+        <v>5876.1432000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11">
+        <v>68482.212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12">
+        <v>76070.592300000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13">
+        <v>91812.097200000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14">
+        <v>415966.99369999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15">
+        <v>376185.31530000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16">
+        <v>355644.78619999997</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17">
+        <v>22472.162400000001</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18">
+        <v>20945.453000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19">
+        <v>21858.642400000001</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20">
+        <v>8161.4591</v>
+      </c>
+    </row>
+    <row r="21" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21">
+        <v>8255.3225000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22">
+        <v>8252.1854000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23">
+        <v>11465.6095</v>
+      </c>
+    </row>
+    <row r="24" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>39</v>
+      </c>
+      <c r="H24">
+        <v>9749.5854999999992</v>
+      </c>
+    </row>
+    <row r="25" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25">
+        <v>9844.7204000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26">
+        <v>12057.7456</v>
+      </c>
+    </row>
+    <row r="27" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27">
+        <v>12102.679400000001</v>
+      </c>
+    </row>
+    <row r="28" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>43</v>
+      </c>
+      <c r="H28">
+        <v>14437.1057</v>
+      </c>
+    </row>
+    <row r="29" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>44</v>
+      </c>
+      <c r="H29">
+        <v>10966.2922</v>
+      </c>
+    </row>
+    <row r="30" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30">
+        <v>11041.8207</v>
+      </c>
+    </row>
+    <row r="31" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>46</v>
+      </c>
+      <c r="H31">
+        <v>11574.048199999999</v>
+      </c>
+    </row>
+    <row r="32" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>47</v>
+      </c>
+      <c r="H32">
+        <v>146405.23759999999</v>
+      </c>
+    </row>
+    <row r="33" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H33">
+        <v>140414.74369999999</v>
+      </c>
+    </row>
+    <row r="34" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>49</v>
+      </c>
+      <c r="H34">
+        <v>150526.46890000001</v>
+      </c>
+    </row>
+    <row r="35" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
+        <v>50</v>
+      </c>
+      <c r="H35">
+        <v>11114.0501</v>
+      </c>
+    </row>
+    <row r="36" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>51</v>
+      </c>
+      <c r="H36">
+        <v>11270.2425</v>
+      </c>
+    </row>
+    <row r="37" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>52</v>
+      </c>
+      <c r="H37">
+        <v>11489.1672</v>
+      </c>
+    </row>
+    <row r="38" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>53</v>
+      </c>
+      <c r="H38">
+        <v>108061.48179999999</v>
+      </c>
+    </row>
+    <row r="39" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
+        <v>54</v>
+      </c>
+      <c r="H39">
+        <v>114581.36719999999</v>
+      </c>
+    </row>
+    <row r="40" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H40">
+        <v>117180.4706</v>
+      </c>
+    </row>
+    <row r="41" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>56</v>
+      </c>
+      <c r="H41">
+        <v>93621.847699999998</v>
+      </c>
+    </row>
+    <row r="42" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
+        <v>57</v>
+      </c>
+      <c r="H42">
+        <v>93572.179199999999</v>
+      </c>
+    </row>
+    <row r="43" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
+        <v>58</v>
+      </c>
+      <c r="H43">
+        <v>94066.012499999997</v>
       </c>
     </row>
   </sheetData>
@@ -593,15 +1051,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98151F63-8C73-C64D-B551-1C8B9D66DF10}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C10"/>
+      <selection activeCell="A6" sqref="A6:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -612,103 +1070,231 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>137.14523333333332</v>
+        <v>534.08280000000002</v>
       </c>
       <c r="C2">
-        <v>3.0774642960290151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3.8624421199546837</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="2">
+        <v>146405.23800000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>5355.0865999999996</v>
+        <v>15596.172400000001</v>
       </c>
       <c r="C3">
-        <v>65.317215750290345</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>788.03543538336555</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="2">
+        <v>140414.74400000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>144757.95853333335</v>
+        <v>382599.03173333331</v>
       </c>
       <c r="C4">
-        <v>7849.7811571914235</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>30668.289784134882</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="2">
+        <v>150526.46900000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>75569.738200000007</v>
+        <v>78788.300500000012</v>
       </c>
       <c r="C5">
-        <v>3851.2502215658369</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11900.014254468426</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="2">
+        <v>11114.0501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>59722.09426666666</v>
+        <f>AVERAGE(H2:H4)</f>
+        <v>145782.15033333332</v>
       </c>
       <c r="C6">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <f>STDEV(H2:H4)</f>
+        <v>5084.5771013104295</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="2">
+        <v>11270.2425</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>11842.476433333331</v>
+        <f>AVERAGE(H5:H7)</f>
+        <v>11291.153266666666</v>
       </c>
       <c r="C7">
-        <v>898.8833893182383</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <f>STDEV(H5:H7)</f>
+        <v>188.43076924972533</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="2">
+        <v>11489.1672</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>38763.979266666669</v>
+        <f>AVERAGE(H8:H10)</f>
+        <v>113274.44</v>
       </c>
       <c r="C8">
-        <v>6310.2056450739401</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <f>STDEV(H8:H10)</f>
+        <v>4697.8754488627092</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="2">
+        <v>108061.482</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
-        <v>30772.651633333327</v>
+        <f>AVERAGE(H11:H13)</f>
+        <v>93753.34646666667</v>
       </c>
       <c r="C9">
-        <v>4367.1110222270918</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <f>STDEV(H11:H13)</f>
+        <v>271.91317782219176</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="2">
+        <v>114581.367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>21410.490333333331</v>
+        <f>AVERAGE(H14,H16,H18)</f>
+        <v>68171.152633333331</v>
       </c>
       <c r="C10">
-        <v>1685.4500277749723</v>
+        <f>STDEV(H14,H16,H18)</f>
+        <v>11033.720807356747</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="2">
+        <v>117180.47100000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="2">
+        <v>93621.847699999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="2">
+        <v>93572.179199999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="2">
+        <v>94066.012499999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14">
+        <v>55899.412199999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15">
+        <v>180.4204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16">
+        <v>71341.169699999999</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17">
+        <v>173.57169999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18">
+        <v>77272.876000000004</v>
       </c>
     </row>
   </sheetData>
@@ -721,7 +1307,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,11 +1316,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -744,11 +1330,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>0</v>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C2">
         <v>137.14523333333332</v>
@@ -757,12 +1343,12 @@
         <v>3.0774642960290151</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C3">
         <v>5355.0865999999996</v>
@@ -772,10 +1358,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
@@ -786,10 +1372,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
@@ -803,15 +1389,21 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>1</v>
+      </c>
+      <c r="C6">
+        <v>21758.752600000003</v>
+      </c>
+      <c r="D6">
+        <v>768.24076767646204</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>5</v>
       </c>
       <c r="C7">
@@ -825,7 +1417,7 @@
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>7.5</v>
       </c>
       <c r="C8">
@@ -839,23 +1431,35 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>10</v>
+      </c>
+      <c r="C9">
+        <v>145782.15033333332</v>
+      </c>
+      <c r="D9">
+        <v>5084.5771013104295</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10">
         <v>1</v>
+      </c>
+      <c r="C10">
+        <v>8222.9890000000014</v>
+      </c>
+      <c r="D10">
+        <v>53.309537557645477</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11">
         <v>5</v>
       </c>
       <c r="C11">
@@ -869,7 +1473,7 @@
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12">
         <v>7.5</v>
       </c>
       <c r="C12">
@@ -883,23 +1487,35 @@
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13">
         <v>10</v>
+      </c>
+      <c r="C13">
+        <v>11291.153266666666</v>
+      </c>
+      <c r="D13">
+        <v>188.43076924972533</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14">
         <v>1</v>
+      </c>
+      <c r="C14">
+        <v>10353.305133333333</v>
+      </c>
+      <c r="D14">
+        <v>964.45757572783066</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15">
         <v>5</v>
       </c>
       <c r="C15">
@@ -913,7 +1529,7 @@
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16">
         <v>7.5</v>
       </c>
       <c r="C16">
@@ -927,23 +1543,35 @@
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17">
         <v>10</v>
+      </c>
+      <c r="C17">
+        <v>113274.44</v>
+      </c>
+      <c r="D17">
+        <v>4697.8754488627092</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18">
         <v>1</v>
+      </c>
+      <c r="C18">
+        <v>12865.843566666668</v>
+      </c>
+      <c r="D18">
+        <v>1360.9383822682871</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19">
         <v>5</v>
       </c>
       <c r="C19">
@@ -957,7 +1585,7 @@
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20">
         <v>7.5</v>
       </c>
       <c r="C20">
@@ -971,23 +1599,35 @@
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21">
         <v>10</v>
+      </c>
+      <c r="C21">
+        <v>93753.34646666667</v>
+      </c>
+      <c r="D21">
+        <v>271.91317782219176</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22">
         <v>1</v>
+      </c>
+      <c r="C22">
+        <v>11194.053699999999</v>
+      </c>
+      <c r="D22">
+        <v>331.24462803304402</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23">
         <v>5</v>
       </c>
       <c r="C23">
@@ -1001,7 +1641,7 @@
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24">
         <v>7.5</v>
       </c>
       <c r="C24">
@@ -1015,8 +1655,14 @@
       <c r="A25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25">
         <v>10</v>
+      </c>
+      <c r="C25">
+        <v>68171.152633333331</v>
+      </c>
+      <c r="D25">
+        <v>11033.720807356747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>